<commit_message>
move files to archive
</commit_message>
<xml_diff>
--- a/TestData/BC/density_mean.xlsx
+++ b/TestData/BC/density_mean.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00073294\Dropbox\projects\1M_Noddies\PETROPHYSICS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Loop3DGKM\TestData\BC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E438F4-C407-49EE-9688-369B1F891991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20010" windowHeight="5910"/>
+    <workbookView xWindow="3015" yWindow="1260" windowWidth="18825" windowHeight="10860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -275,7 +276,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -291,18 +292,12 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -317,12 +312,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -332,8 +324,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{C174C7D5-FD17-4337-9953-860C08E04BAB}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -607,37 +627,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="2">
         <v>2.800497</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>2.8759329999999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>2.7211889999999999</v>
       </c>
     </row>
@@ -645,23 +667,23 @@
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>2.5945469999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>2.6608700000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>4.5511429999999997</v>
       </c>
     </row>
@@ -669,23 +691,23 @@
       <c r="A7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>2.7926899999999999</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>2.63734</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>2.6562950000000001</v>
       </c>
     </row>
@@ -693,23 +715,23 @@
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>2.62</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>2.388347</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>2.6186950000000002</v>
       </c>
     </row>
@@ -717,23 +739,23 @@
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>2.62127</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>2.782734</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>2.8516080000000001</v>
       </c>
     </row>
@@ -741,23 +763,23 @@
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>2.716523</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>3.0854539999999999</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>2.7724850000000001</v>
       </c>
     </row>
@@ -765,23 +787,23 @@
       <c r="A19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>2.9502280000000001</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>2.6125929999999999</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>3.0043350000000002</v>
       </c>
     </row>
@@ -789,23 +811,23 @@
       <c r="A22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <v>2.7011910000000001</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>2.6915770000000001</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>2.76</v>
       </c>
     </row>
@@ -813,23 +835,23 @@
       <c r="A25" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>3.027914</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>2.9104589999999999</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>2.710769</v>
       </c>
     </row>
@@ -837,23 +859,23 @@
       <c r="A28" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>2.7416420000000001</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>2.7139120000000001</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>2.793914</v>
       </c>
     </row>
@@ -861,23 +883,23 @@
       <c r="A31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
         <v>2.871775</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>3.4099930000000001</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>2.7389649999999999</v>
       </c>
     </row>
@@ -885,23 +907,23 @@
       <c r="A34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="2">
         <v>2.7825839999999999</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>2.894892</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>2.8144610000000001</v>
       </c>
     </row>
@@ -909,23 +931,23 @@
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="2">
         <v>2.9829919999999999</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>2.8439410000000001</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="2">
         <v>3.307124</v>
       </c>
     </row>
@@ -933,23 +955,23 @@
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="2">
         <v>2.6867049999999999</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="2">
         <v>2.8197800000000002</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="2">
         <v>2.3784109999999998</v>
       </c>
     </row>
@@ -957,23 +979,23 @@
       <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="2">
         <v>2.6990419999999999</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="2">
         <v>2.6985540000000001</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="2">
         <v>2.8510759999999999</v>
       </c>
     </row>
@@ -981,23 +1003,23 @@
       <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="2">
         <v>2.7391770000000002</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <v>2.8400240000000001</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="2">
         <v>2.648774</v>
       </c>
     </row>
@@ -1005,23 +1027,23 @@
       <c r="A49" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="2">
         <v>3.1943790000000001</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <v>2.6805699999999999</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="2">
         <v>2.630833</v>
       </c>
     </row>
@@ -1029,23 +1051,23 @@
       <c r="A52" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="2">
         <v>2.6916449999999998</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="2">
         <v>2.6226720000000001</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="2">
         <v>2.7380620000000002</v>
       </c>
     </row>
@@ -1053,23 +1075,23 @@
       <c r="A55" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="2">
         <v>2.7996759999999998</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="2">
         <v>2.7138610000000001</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="2">
         <v>2.6877909999999998</v>
       </c>
     </row>
@@ -1077,23 +1099,23 @@
       <c r="A58" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="2">
         <v>2.6289709999999999</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="2">
         <v>3.154741</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B60" s="2">
         <v>2.9602200000000001</v>
       </c>
     </row>
@@ -1101,23 +1123,23 @@
       <c r="A61" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61" s="2">
         <v>3.1139169999999998</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B62" s="3">
+      <c r="B62" s="2">
         <v>2.6858240000000002</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B63" s="2">
         <v>2.6444700000000001</v>
       </c>
     </row>
@@ -1125,23 +1147,23 @@
       <c r="A64" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64" s="2">
         <v>2.6045379999999998</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="3">
+      <c r="B65" s="2">
         <v>2.6327050000000001</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B66" s="2">
         <v>2.728119</v>
       </c>
     </row>
@@ -1149,23 +1171,23 @@
       <c r="A67" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67" s="2">
         <v>2.7602280000000001</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B68" s="2">
         <v>2.6590470000000002</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B69" s="2">
         <v>2.41</v>
       </c>
     </row>
@@ -1173,23 +1195,23 @@
       <c r="A70" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="2">
         <v>2.7128549999999998</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B71" s="2">
         <v>2.6127379999999998</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B72" s="3">
+      <c r="B72" s="2">
         <v>2.6626560000000001</v>
       </c>
     </row>
@@ -1197,23 +1219,23 @@
       <c r="A73" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="2">
         <v>2.5746099999999998</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B74" s="3">
+      <c r="B74" s="2">
         <v>2.6896119999999999</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B75" s="3">
+      <c r="B75" s="2">
         <v>2.7212730000000001</v>
       </c>
     </row>
@@ -1221,23 +1243,23 @@
       <c r="A76" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76" s="2">
         <v>2.701965</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B77" s="3">
+      <c r="B77" s="2">
         <v>2.771579</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B78" s="3">
+      <c r="B78" s="2">
         <v>2.7552669999999999</v>
       </c>
     </row>
@@ -1245,23 +1267,23 @@
       <c r="A79" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="2">
         <v>2.7797149999999999</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B80" s="3">
+      <c r="B80" s="2">
         <v>2.8593470000000001</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B81" s="3">
+      <c r="B81" s="2">
         <v>2.8083330000000002</v>
       </c>
     </row>
@@ -1269,7 +1291,7 @@
       <c r="A82" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82" s="2">
         <v>2.8614630000000001</v>
       </c>
     </row>
@@ -1358,7 +1380,7 @@
       <c r="A110" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A1:E82">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:E82">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>